<commit_message>
Update HGL-0200 Calibration datasheet.xlsx
</commit_message>
<xml_diff>
--- a/SonoRover One/software/src/config/hydrophones/HGL-0200 Calibration datasheet.xlsx
+++ b/SonoRover One/software/src/config/hydrophones/HGL-0200 Calibration datasheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://radbouduniversiteit-my.sharepoint.com/personal/margely_cornelissen_ru_nl/Documents/Documenten/GitHub/repositories/Radboud-FUS-measurement-kit/SonoRover One/software/src/config/hydrophones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{F0885107-4186-4DB7-B324-BAF8E1B0D248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFA587AE-12EC-4DE5-9F85-B711087BD0B5}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{F0885107-4186-4DB7-B324-BAF8E1B0D248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0E261B7-C8F3-4165-9D0B-D215E5051A7E}"/>
   <bookViews>
-    <workbookView xWindow="-25693" yWindow="-60" windowWidth="25786" windowHeight="15467" xr2:uid="{D9C677B7-77BB-444A-8CBB-DB80A4FE56DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D9C677B7-77BB-444A-8CBB-DB80A4FE56DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,7 +436,7 @@
         <v>0.25</v>
       </c>
       <c r="B2" s="1">
-        <v>2.4790000000000001E-4</v>
+        <v>2.4789999999999999E-7</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -445,7 +445,7 @@
         <v>0.3</v>
       </c>
       <c r="B3" s="1">
-        <v>2.8959999999999999E-4</v>
+        <v>2.896E-7</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -454,7 +454,7 @@
         <v>0.35</v>
       </c>
       <c r="B4" s="1">
-        <v>2.812E-4</v>
+        <v>2.812E-7</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -463,7 +463,7 @@
         <v>0.4</v>
       </c>
       <c r="B5" s="1">
-        <v>2.8659999999999997E-4</v>
+        <v>2.8659999999999999E-7</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -472,7 +472,7 @@
         <v>0.45</v>
       </c>
       <c r="B6" s="1">
-        <v>2.8439999999999997E-4</v>
+        <v>2.8439999999999998E-7</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -481,7 +481,7 @@
         <v>0.5</v>
       </c>
       <c r="B7" s="1">
-        <v>2.6909999999999998E-4</v>
+        <v>2.6909999999999999E-7</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -490,7 +490,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="B8" s="1">
-        <v>2.6340000000000001E-4</v>
+        <v>2.6339999999999999E-7</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -499,7 +499,7 @@
         <v>0.6</v>
       </c>
       <c r="B9" s="1">
-        <v>2.5680000000000001E-4</v>
+        <v>2.5680000000000002E-7</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -508,7 +508,7 @@
         <v>0.65</v>
       </c>
       <c r="B10" s="1">
-        <v>2.5510000000000002E-4</v>
+        <v>2.551E-7</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -517,7 +517,7 @@
         <v>0.7</v>
       </c>
       <c r="B11" s="1">
-        <v>2.5119999999999998E-4</v>
+        <v>2.5120000000000003E-7</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -526,7 +526,7 @@
         <v>0.75</v>
       </c>
       <c r="B12" s="1">
-        <v>2.4469999999999998E-4</v>
+        <v>2.4470000000000001E-7</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -535,7 +535,7 @@
         <v>0.8</v>
       </c>
       <c r="B13" s="1">
-        <v>2.3910000000000001E-4</v>
+        <v>2.3910000000000002E-7</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -544,7 +544,7 @@
         <v>0.85</v>
       </c>
       <c r="B14" s="1">
-        <v>2.2660000000000001E-4</v>
+        <v>2.266E-7</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -553,7 +553,7 @@
         <v>0.9</v>
       </c>
       <c r="B15" s="1">
-        <v>2.1599999999999999E-4</v>
+        <v>2.16E-7</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -562,7 +562,7 @@
         <v>0.95</v>
       </c>
       <c r="B16" s="1">
-        <v>2.0560000000000001E-4</v>
+        <v>2.0559999999999999E-7</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -571,7 +571,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="1">
-        <v>1.9689999999999999E-4</v>
+        <v>1.969E-7</v>
       </c>
       <c r="D17" s="1"/>
     </row>

</xml_diff>